<commit_message>
Correccion de errores en el package y adicion de link de github
</commit_message>
<xml_diff>
--- a/out/production/Hoja-de-trabajo-3/Gráficas.xlsx
+++ b/out/production/Hoja-de-trabajo-3/Gráficas.xlsx
@@ -1,17 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Avila\OneDrive\Documentos\UVG\Segundo año 2021\Algoritmos y estructuras de datos\HDT3\Hoja-de-trabajo-3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5DC47A-216E-4F24-8356-ED83D0D445A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="10752" yWindow="234" windowWidth="12288" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">Merge </t>
   </si>
@@ -65,29 +85,37 @@
   </si>
   <si>
     <t>O(n^2)</t>
+  </si>
+  <si>
+    <t>Datos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -97,11 +125,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -115,49 +149,49 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -168,11 +202,17 @@
     <xdr:ext cx="4581525" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png" title="Imagen"/>
+        <xdr:cNvPr id="2" name="image10.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -196,11 +236,17 @@
     <xdr:ext cx="4581525" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image15.png" title="Imagen"/>
+        <xdr:cNvPr id="3" name="image15.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -217,23 +263,33 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
+      <xdr:colOff>971550</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:rowOff>184785</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4572000" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.png" title="Imagen"/>
+        <xdr:cNvPr id="4" name="image13.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13178790" y="2760345"/>
+          <a:ext cx="4572000" cy="2752725"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -252,11 +308,17 @@
     <xdr:ext cx="4581525" cy="2743200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Imagen"/>
+        <xdr:cNvPr id="5" name="image5.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -280,11 +342,17 @@
     <xdr:ext cx="4581525" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Imagen"/>
+        <xdr:cNvPr id="6" name="image2.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -308,11 +376,17 @@
     <xdr:ext cx="4581525" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Imagen"/>
+        <xdr:cNvPr id="7" name="image3.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -336,11 +410,17 @@
     <xdr:ext cx="4581525" cy="2743200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image17.png" title="Imagen"/>
+        <xdr:cNvPr id="8" name="image17.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -357,23 +437,33 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:colOff>283845</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4581525" cy="2743200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.png" title="Imagen"/>
+        <xdr:cNvPr id="9" name="image14.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11500485" y="12104370"/>
+          <a:ext cx="4581525" cy="2743200"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -392,11 +482,17 @@
     <xdr:ext cx="4581525" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Imagen"/>
+        <xdr:cNvPr id="10" name="image8.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -420,11 +516,17 @@
     <xdr:ext cx="4581525" cy="2743200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Imagen"/>
+        <xdr:cNvPr id="11" name="image1.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -448,11 +550,17 @@
     <xdr:ext cx="4581525" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image16.png" title="Imagen"/>
+        <xdr:cNvPr id="12" name="image16.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -476,11 +584,17 @@
     <xdr:ext cx="4724400" cy="2962275"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Imagen"/>
+        <xdr:cNvPr id="13" name="image11.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -504,11 +618,17 @@
     <xdr:ext cx="4581525" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Imagen"/>
+        <xdr:cNvPr id="14" name="image6.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -532,11 +652,17 @@
     <xdr:ext cx="4581525" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Imagen"/>
+        <xdr:cNvPr id="15" name="image12.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -560,11 +686,17 @@
     <xdr:ext cx="4572000" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Imagen"/>
+        <xdr:cNvPr id="16" name="image7.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -588,11 +720,17 @@
     <xdr:ext cx="4572000" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Imagen"/>
+        <xdr:cNvPr id="17" name="image4.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -616,11 +754,17 @@
     <xdr:ext cx="4581525" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Imagen"/>
+        <xdr:cNvPr id="18" name="image9.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -638,7 +782,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -828,25 +972,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection sqref="A1:K11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="1" min="7" max="7" width="16.71"/>
-    <col customWidth="1" min="9" max="9" width="16.86"/>
+    <col min="7" max="7" width="16.71875" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -894,39 +1045,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2">
-        <v>119.0</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3">
-        <v>8263.0</v>
+        <v>8263</v>
       </c>
       <c r="E2" s="3">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="F2" s="2">
-        <v>1103.0</v>
+        <v>1103</v>
       </c>
       <c r="G2" s="3">
-        <v>178.0</v>
+        <v>178</v>
       </c>
       <c r="H2" s="3">
-        <v>2101.0</v>
+        <v>2101</v>
       </c>
       <c r="I2" s="3">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="J2" s="3">
-        <v>124.0</v>
+        <v>124</v>
       </c>
       <c r="K2" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="5" t="s">
@@ -945,524 +1096,525 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="B3" s="3">
-        <v>226.0</v>
+        <v>226</v>
       </c>
       <c r="C3" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3">
-        <v>9733.0</v>
+        <v>9733</v>
       </c>
       <c r="E3" s="3">
-        <v>151.0</v>
+        <v>151</v>
       </c>
       <c r="F3" s="2">
-        <v>3365.0</v>
+        <v>3365</v>
       </c>
       <c r="G3" s="3">
-        <v>787.0</v>
+        <v>787</v>
       </c>
       <c r="H3" s="3">
-        <v>3941.0</v>
+        <v>3941</v>
       </c>
       <c r="I3" s="3">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="J3" s="3">
-        <v>263.0</v>
+        <v>263</v>
       </c>
       <c r="K3" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="7">
-        <f t="shared" ref="M3:M12" si="1">A2*LOG(A2,2)</f>
-        <v>282.1928095</v>
+        <f t="shared" ref="M3:M12" si="0">A2*LOG(A2,2)</f>
+        <v>282.1928094887362</v>
       </c>
       <c r="N3" s="8">
-        <f t="shared" ref="N3:N12" si="2">A2</f>
+        <f t="shared" ref="N3:N12" si="1">A2</f>
         <v>50</v>
       </c>
       <c r="O3" s="8">
-        <f t="shared" ref="O3:O12" si="3">POWER(B2,2)</f>
+        <f t="shared" ref="O3:O12" si="2">POWER(B2,2)</f>
         <v>14161</v>
       </c>
       <c r="P3" s="8">
-        <f t="shared" ref="P3:P12" si="4">POWER(A2,2)</f>
+        <f t="shared" ref="P3:P12" si="3">POWER(A2,2)</f>
         <v>2500</v>
       </c>
       <c r="Q3" s="5">
-        <v>2500.0</v>
+        <v>2500</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="B4" s="2">
-        <v>1258.0</v>
+        <v>1258</v>
       </c>
       <c r="C4" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3">
-        <v>9716.0</v>
+        <v>9716</v>
       </c>
       <c r="E4" s="3">
-        <v>704.0</v>
+        <v>704</v>
       </c>
       <c r="F4" s="2">
-        <v>62618.0</v>
+        <v>62618</v>
       </c>
       <c r="G4" s="3">
-        <v>13531.0</v>
+        <v>13531</v>
       </c>
       <c r="H4" s="3">
-        <v>190815.0</v>
+        <v>190815</v>
       </c>
       <c r="I4" s="3">
-        <v>183.0</v>
+        <v>183</v>
       </c>
       <c r="J4" s="3">
-        <v>3725.0</v>
+        <v>3725</v>
       </c>
       <c r="K4" s="3">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="7">
+        <f t="shared" si="0"/>
+        <v>664.38561897747252</v>
+      </c>
+      <c r="N4" s="8">
         <f t="shared" si="1"/>
-        <v>664.385619</v>
-      </c>
-      <c r="N4" s="8">
+        <v>100</v>
+      </c>
+      <c r="O4" s="8">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="O4" s="8">
+        <v>51076</v>
+      </c>
+      <c r="P4" s="8">
         <f t="shared" si="3"/>
-        <v>51076</v>
-      </c>
-      <c r="P4" s="8">
-        <f t="shared" si="4"/>
         <v>10000</v>
       </c>
       <c r="Q4" s="5">
-        <v>10000.0</v>
+        <v>10000</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="B5" s="2">
-        <v>2702.0</v>
+        <v>2702</v>
       </c>
       <c r="C5" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3">
-        <v>9063.0</v>
+        <v>9063</v>
       </c>
       <c r="E5" s="3">
-        <v>2179.0</v>
+        <v>2179</v>
       </c>
       <c r="F5" s="3">
-        <v>232000.0</v>
+        <v>232000</v>
       </c>
       <c r="G5" s="3">
-        <v>46601.0</v>
+        <v>46601</v>
       </c>
       <c r="H5" s="3">
-        <v>255817.0</v>
+        <v>255817</v>
       </c>
       <c r="I5" s="3">
-        <v>340.0</v>
+        <v>340</v>
       </c>
       <c r="J5" s="3">
-        <v>12575.0</v>
+        <v>12575</v>
       </c>
       <c r="K5" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="7">
+        <f t="shared" si="0"/>
+        <v>4482.8921423310439</v>
+      </c>
+      <c r="N5" s="8">
         <f t="shared" si="1"/>
-        <v>4482.892142</v>
-      </c>
-      <c r="N5" s="8">
+        <v>500</v>
+      </c>
+      <c r="O5" s="8">
         <f t="shared" si="2"/>
-        <v>500</v>
-      </c>
-      <c r="O5" s="8">
+        <v>1582564</v>
+      </c>
+      <c r="P5" s="8">
         <f t="shared" si="3"/>
-        <v>1582564</v>
-      </c>
-      <c r="P5" s="8">
-        <f t="shared" si="4"/>
         <v>250000</v>
       </c>
       <c r="Q5" s="5">
-        <v>250000.0</v>
+        <v>250000</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6">
-        <v>1200.0</v>
+        <v>1200</v>
       </c>
       <c r="B6" s="2">
-        <v>3434.0</v>
+        <v>3434</v>
       </c>
       <c r="C6" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
-        <v>11805.0</v>
+        <v>11805</v>
       </c>
       <c r="E6" s="3">
-        <v>2937.0</v>
+        <v>2937</v>
       </c>
       <c r="F6" s="2">
-        <v>325000.0</v>
+        <v>325000</v>
       </c>
       <c r="G6" s="3">
-        <v>60572.0</v>
+        <v>60572</v>
       </c>
       <c r="H6" s="3">
-        <v>359299.0</v>
+        <v>359299</v>
       </c>
       <c r="I6" s="3">
-        <v>411.0</v>
+        <v>411</v>
       </c>
       <c r="J6" s="3">
-        <v>18040.0</v>
+        <v>18040</v>
       </c>
       <c r="K6" s="3">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="7">
+        <f t="shared" si="0"/>
+        <v>9965.7842846620879</v>
+      </c>
+      <c r="N6" s="8">
         <f t="shared" si="1"/>
-        <v>9965.784285</v>
-      </c>
-      <c r="N6" s="8">
+        <v>1000</v>
+      </c>
+      <c r="O6" s="8">
         <f t="shared" si="2"/>
-        <v>1000</v>
-      </c>
-      <c r="O6" s="8">
+        <v>7300804</v>
+      </c>
+      <c r="P6" s="8">
         <f t="shared" si="3"/>
-        <v>7300804</v>
-      </c>
-      <c r="P6" s="8">
-        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
       <c r="Q6" s="5">
-        <v>1000000.0</v>
+        <v>1000000</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="B7" s="2">
-        <v>3399.0</v>
+        <v>3399</v>
       </c>
       <c r="C7" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3">
-        <v>11639.0</v>
+        <v>11639</v>
       </c>
       <c r="E7" s="3">
-        <v>2421.0</v>
+        <v>2421</v>
       </c>
       <c r="F7" s="3">
-        <v>509000.0</v>
+        <v>509000</v>
       </c>
       <c r="G7" s="3">
-        <v>91518.0</v>
+        <v>91518</v>
       </c>
       <c r="H7" s="3">
-        <v>952600.0</v>
+        <v>952600</v>
       </c>
       <c r="I7" s="3">
-        <v>494.0</v>
+        <v>494</v>
       </c>
       <c r="J7" s="3">
-        <v>27287.0</v>
+        <v>27287</v>
       </c>
       <c r="K7" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="7">
+        <f t="shared" si="0"/>
+        <v>12274.582428595058</v>
+      </c>
+      <c r="N7" s="8">
         <f t="shared" si="1"/>
-        <v>12274.58243</v>
-      </c>
-      <c r="N7" s="8">
+        <v>1200</v>
+      </c>
+      <c r="O7" s="8">
         <f t="shared" si="2"/>
-        <v>1200</v>
-      </c>
-      <c r="O7" s="8">
+        <v>11792356</v>
+      </c>
+      <c r="P7" s="8">
         <f t="shared" si="3"/>
-        <v>11792356</v>
-      </c>
-      <c r="P7" s="8">
-        <f t="shared" si="4"/>
         <v>1440000</v>
       </c>
       <c r="Q7" s="5">
-        <v>1440000.0</v>
+        <v>1440000</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="B8" s="2">
-        <v>3788.0</v>
+        <v>3788</v>
       </c>
       <c r="C8" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3">
-        <v>10960.0</v>
+        <v>10960</v>
       </c>
       <c r="E8" s="3">
-        <v>3167.0</v>
+        <v>3167</v>
       </c>
       <c r="F8" s="2">
-        <v>847000.0</v>
+        <v>847000</v>
       </c>
       <c r="G8" s="3">
-        <v>158596.0</v>
+        <v>158596</v>
       </c>
       <c r="H8" s="3">
-        <v>839213.0</v>
+        <v>839213</v>
       </c>
       <c r="I8" s="3">
-        <v>762.0</v>
+        <v>762</v>
       </c>
       <c r="J8" s="3">
-        <v>38062.0</v>
+        <v>38062</v>
       </c>
       <c r="K8" s="3">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="7">
+        <f t="shared" si="0"/>
+        <v>15826.120178074865</v>
+      </c>
+      <c r="N8" s="8">
         <f t="shared" si="1"/>
-        <v>15826.12018</v>
-      </c>
-      <c r="N8" s="8">
+        <v>1500</v>
+      </c>
+      <c r="O8" s="8">
         <f t="shared" si="2"/>
-        <v>1500</v>
-      </c>
-      <c r="O8" s="8">
+        <v>11553201</v>
+      </c>
+      <c r="P8" s="8">
         <f t="shared" si="3"/>
-        <v>11553201</v>
-      </c>
-      <c r="P8" s="8">
-        <f t="shared" si="4"/>
         <v>2250000</v>
       </c>
       <c r="Q8" s="5">
-        <v>2250000.0</v>
+        <v>2250000</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6">
-        <v>2200.0</v>
+        <v>2200</v>
       </c>
       <c r="B9" s="3">
-        <v>8796.0</v>
+        <v>8796</v>
       </c>
       <c r="C9" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D9" s="3">
-        <v>16395.0</v>
+        <v>16395</v>
       </c>
       <c r="E9" s="3">
-        <v>3518.0</v>
+        <v>3518</v>
       </c>
       <c r="F9" s="2">
-        <v>1045000.0</v>
+        <v>1045000</v>
       </c>
       <c r="G9" s="3">
-        <v>200366.0</v>
+        <v>200366</v>
       </c>
       <c r="H9" s="3">
-        <v>1294987.0</v>
+        <v>1294987</v>
       </c>
       <c r="I9" s="3">
-        <v>799.0</v>
+        <v>799</v>
       </c>
       <c r="J9" s="3">
-        <v>56889.0</v>
+        <v>56889</v>
       </c>
       <c r="K9" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="7">
+        <f t="shared" si="0"/>
+        <v>21931.568569324176</v>
+      </c>
+      <c r="N9" s="8">
         <f t="shared" si="1"/>
-        <v>21931.56857</v>
-      </c>
-      <c r="N9" s="8">
+        <v>2000</v>
+      </c>
+      <c r="O9" s="8">
         <f t="shared" si="2"/>
-        <v>2000</v>
-      </c>
-      <c r="O9" s="8">
+        <v>14348944</v>
+      </c>
+      <c r="P9" s="8">
         <f t="shared" si="3"/>
-        <v>14348944</v>
-      </c>
-      <c r="P9" s="8">
-        <f t="shared" si="4"/>
         <v>4000000</v>
       </c>
       <c r="Q9" s="5">
-        <v>4000000.0</v>
+        <v>4000000</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6">
-        <v>2500.0</v>
+        <v>2500</v>
       </c>
       <c r="B10" s="2">
-        <v>5878.0</v>
+        <v>5878</v>
       </c>
       <c r="C10" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3">
-        <v>16987.0</v>
+        <v>16987</v>
       </c>
       <c r="E10" s="3">
-        <v>4082.0</v>
+        <v>4082</v>
       </c>
       <c r="F10" s="3">
-        <v>1463074.0</v>
+        <v>1463074</v>
       </c>
       <c r="G10" s="3">
-        <v>253164.0</v>
+        <v>253164</v>
       </c>
       <c r="H10" s="3">
-        <v>1400058.0</v>
+        <v>1400058</v>
       </c>
       <c r="I10" s="3">
-        <v>907.0</v>
+        <v>907</v>
       </c>
       <c r="J10" s="3">
-        <v>80982.0</v>
+        <v>80982</v>
       </c>
       <c r="K10" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="7">
+        <f t="shared" si="0"/>
+        <v>24427.233178506449</v>
+      </c>
+      <c r="N10" s="8">
         <f t="shared" si="1"/>
-        <v>24427.23318</v>
-      </c>
-      <c r="N10" s="8">
+        <v>2200</v>
+      </c>
+      <c r="O10" s="8">
         <f t="shared" si="2"/>
-        <v>2200</v>
-      </c>
-      <c r="O10" s="8">
+        <v>77369616</v>
+      </c>
+      <c r="P10" s="8">
         <f t="shared" si="3"/>
-        <v>77369616</v>
-      </c>
-      <c r="P10" s="8">
-        <f t="shared" si="4"/>
         <v>4840000</v>
       </c>
       <c r="Q10" s="5">
-        <v>4840000.0</v>
+        <v>4840000</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="B11" s="3">
-        <v>11996.0</v>
+        <v>11996</v>
       </c>
       <c r="C11" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="D11" s="3">
-        <v>20475.0</v>
+        <v>20475</v>
       </c>
       <c r="E11" s="3">
-        <v>4439.0</v>
+        <v>4439</v>
       </c>
       <c r="F11" s="2">
-        <v>2015000.0</v>
+        <v>2015000</v>
       </c>
       <c r="G11" s="3">
-        <v>350341.0</v>
+        <v>350341</v>
       </c>
       <c r="H11" s="3">
-        <v>2394773.0</v>
+        <v>2394773</v>
       </c>
       <c r="I11" s="3">
-        <v>992.0</v>
+        <v>992</v>
       </c>
       <c r="J11" s="3">
-        <v>84381.0</v>
+        <v>84381</v>
       </c>
       <c r="K11" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="7">
+        <f t="shared" si="0"/>
+        <v>28219.28094887362</v>
+      </c>
+      <c r="N11" s="8">
         <f t="shared" si="1"/>
-        <v>28219.28095</v>
-      </c>
-      <c r="N11" s="8">
+        <v>2500</v>
+      </c>
+      <c r="O11" s="8">
         <f t="shared" si="2"/>
-        <v>2500</v>
-      </c>
-      <c r="O11" s="8">
+        <v>34550884</v>
+      </c>
+      <c r="P11" s="8">
         <f t="shared" si="3"/>
-        <v>34550884</v>
-      </c>
-      <c r="P11" s="8">
-        <f t="shared" si="4"/>
         <v>6250000</v>
       </c>
       <c r="Q11" s="5">
-        <v>6250000.0</v>
+        <v>6250000</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="L12" s="4"/>
       <c r="M12" s="7">
+        <f t="shared" si="0"/>
+        <v>34652.240356149727</v>
+      </c>
+      <c r="N12" s="8">
         <f t="shared" si="1"/>
-        <v>34652.24036</v>
-      </c>
-      <c r="N12" s="8">
+        <v>3000</v>
+      </c>
+      <c r="O12" s="8">
         <f t="shared" si="2"/>
-        <v>3000</v>
-      </c>
-      <c r="O12" s="8">
+        <v>143904016</v>
+      </c>
+      <c r="P12" s="8">
         <f t="shared" si="3"/>
-        <v>143904016</v>
-      </c>
-      <c r="P12" s="8">
-        <f t="shared" si="4"/>
         <v>9000000</v>
       </c>
       <c r="Q12" s="5">
-        <v>9000000.0</v>
+        <v>9000000</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>